<commit_message>
Updated README files and started NMDS for Flying/Not Flying.
</commit_message>
<xml_diff>
--- a/data/raw/Survival/Survival_run_list.xlsx
+++ b/data/raw/Survival/Survival_run_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t xml:space="preserve">Survival box</t>
   </si>
@@ -46,26 +46,40 @@
     <t xml:space="preserve">0101-0200</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Sv_0158 and Sv_0104 were </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">halved with extract left in vial.</t>
-    </r>
+    <t xml:space="preserve">Sv_0158 and Sv_0104 were halved with extract left in vial.</t>
   </si>
   <si>
     <t xml:space="preserve">0001-0100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In cooling room, in inserts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0201-0300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracted, concentrated, in inserts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0301-0400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extracted and concentrated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0401-0500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0501-0600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0601-0650</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In box along with blanks, derivatised bee sample and cleaned bee sample before derivatisation.</t>
   </si>
 </sst>
 </file>
@@ -76,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,11 +119,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,12 +128,68 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -153,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,24 +227,64 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -203,13 +308,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.52"/>
@@ -226,79 +331,201 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="n">
+      <c r="B2" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="n">
+      <c r="B5" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="D8" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="16"/>
+      <c r="C23" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="24">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="C2:C4"/>
@@ -308,6 +535,21 @@
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>